<commit_message>
Cambio de las horas
</commit_message>
<xml_diff>
--- a/Excel Anteproyecto.xlsx
+++ b/Excel Anteproyecto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FX506\Desktop\Anteproyecto DAM Laura Salas Ávila\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58259B40-C19F-4337-8893-B679B2FC5E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{242F06FE-0F40-4FC1-913C-1AD71DD9C7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4A74DD1-E16E-4E57-8377-910EEAB9A2CB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>ID</t>
   </si>
@@ -72,20 +72,20 @@
     <t>Alta</t>
   </si>
   <si>
-    <t>1-2 h</t>
-  </si>
-  <si>
-    <t>?</t>
+    <t>Configuración y creación del proyecto</t>
   </si>
   <si>
     <t>Descargué flutter y me encargué ya de configurar 
 todo en VSC, he creado un proyecto por defecto flutter y lo he subido a GitHub</t>
   </si>
   <si>
-    <t>1-2 h ?</t>
+    <t>Configuración de Odoo</t>
   </si>
   <si>
     <t>Hay que usar Odoo y configurarlo</t>
+  </si>
+  <si>
+    <t>Intentar realizar la conexión</t>
   </si>
   <si>
     <t>He visto que hay algunos videos en youtube y
@@ -105,15 +105,6 @@
     <t>Crítica</t>
   </si>
   <si>
-    <t>3 h ?</t>
-  </si>
-  <si>
-    <t>2-3 h ?</t>
-  </si>
-  <si>
-    <t>depende ?</t>
-  </si>
-  <si>
     <t>La típica de inicio de sesión</t>
   </si>
   <si>
@@ -136,12 +127,6 @@
     <t>Desarrollar las otras pantallas</t>
   </si>
   <si>
-    <t>3-4 h ?</t>
-  </si>
-  <si>
-    <t>Serán bastantes</t>
-  </si>
-  <si>
     <t>Ver como empezar a poner código</t>
   </si>
   <si>
@@ -152,9 +137,6 @@
     <t>Organización del código, carpetas…..</t>
   </si>
   <si>
-    <t>1-2 h?</t>
-  </si>
-  <si>
     <t>Organizar e intentar mantener el código limpio
 y una estructura ordenada con carpetas, etc..</t>
   </si>
@@ -170,9 +152,6 @@
   </si>
   <si>
     <t>Tener todo subido en GitHub</t>
-  </si>
-  <si>
-    <t>Menos de unos minutos</t>
   </si>
   <si>
     <t>Carpeta con excel/anteproyecto + el proyecto 
@@ -181,9 +160,6 @@
   </si>
   <si>
     <t>Documento Word del proyecto</t>
-  </si>
-  <si>
-    <t>Bastantes horas</t>
   </si>
   <si>
     <t>Ir escribiendo a medida que avanzo el proyecto,
@@ -223,14 +199,37 @@
     <t>Se me olvidaba, poner el código y explicarlo un poco</t>
   </si>
   <si>
-    <t>Configuración y creación del proyecto 
-con Flutter</t>
-  </si>
-  <si>
-    <t>Instalación y configuración de Odoo</t>
-  </si>
-  <si>
-    <t>Realizar la conexión entre Odoo y Flutter</t>
+    <t>2 h</t>
+  </si>
+  <si>
+    <t>4 h</t>
+  </si>
+  <si>
+    <t>6 h</t>
+  </si>
+  <si>
+    <t>3 h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 h </t>
+  </si>
+  <si>
+    <t>7 h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 h </t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>0.5 h</t>
+  </si>
+  <si>
+    <t>5h</t>
   </si>
 </sst>
 </file>
@@ -314,6 +313,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -616,7 +619,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,7 +629,7 @@
     <col min="3" max="3" width="12.44140625" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" customWidth="1"/>
     <col min="5" max="5" width="36.5546875" customWidth="1"/>
-    <col min="6" max="6" width="46.21875" customWidth="1"/>
+    <col min="6" max="6" width="43.77734375" customWidth="1"/>
     <col min="8" max="8" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -654,20 +657,18 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>57</v>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -675,19 +676,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -695,17 +694,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
@@ -718,7 +715,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -729,16 +726,14 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -749,16 +744,14 @@
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -769,13 +762,11 @@
         <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="H8" t="s">
         <v>4</v>
@@ -789,70 +780,64 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
         <v>7</v>
@@ -866,24 +851,22 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H14" t="s">
         <v>8</v>
@@ -894,22 +877,20 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -920,126 +901,121 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="D21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>

</xml_diff>